<commit_message>
done Eng Report Form
</commit_message>
<xml_diff>
--- a/public/Format.xlsx
+++ b/public/Format.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C39D3F6-D8D4-4013-9EF2-8E29F6325F6C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1EAB0C-EF71-48AC-B7C1-2EF2E7662421}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -155,12 +155,6 @@
       <t>ゲツ</t>
     </rPh>
     <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t xml:space="preserve">jupiter ver4.1.1 : -
-JPT-OPTISHAPE : -
-Other : -
-</t>
   </si>
   <si>
     <t>土</t>
@@ -213,9 +207,6 @@
       <t>ジ</t>
     </rPh>
     <phoneticPr fontId="0"/>
-  </si>
-  <si>
-    <t>jupiter ver4.1.1</t>
   </si>
   <si>
     <t>日付</t>
@@ -1449,7 +1440,7 @@
   <dimension ref="B1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1469,7 +1460,7 @@
     </row>
     <row r="2" spans="2:7">
       <c r="B2" s="64" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" s="64"/>
       <c r="D2" s="29"/>
@@ -1481,7 +1472,7 @@
     </row>
     <row r="4" spans="2:7" ht="15" thickBot="1">
       <c r="B4" s="31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>32</v>
@@ -1509,7 +1500,7 @@
       </c>
       <c r="D6" s="37"/>
     </row>
-    <row r="7" spans="2:7" ht="55.2">
+    <row r="7" spans="2:7">
       <c r="B7" s="33">
         <f t="shared" ref="B7:B11" si="0">B6+1</f>
         <v>3</v>
@@ -1517,11 +1508,9 @@
       <c r="C7" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="55.2">
+      <c r="D7" s="35"/>
+    </row>
+    <row r="8" spans="2:7">
       <c r="B8" s="33">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1529,11 +1518,9 @@
       <c r="C8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="55.2">
+      <c r="D8" s="35"/>
+    </row>
+    <row r="9" spans="2:7">
       <c r="B9" s="33">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1541,11 +1528,9 @@
       <c r="C9" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="55.2">
+      <c r="D9" s="35"/>
+    </row>
+    <row r="10" spans="2:7">
       <c r="B10" s="33">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1553,9 +1538,7 @@
       <c r="C10" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="35" t="s">
-        <v>36</v>
-      </c>
+      <c r="D10" s="35"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="33">
@@ -1563,13 +1546,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="35"/>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="62"/>
       <c r="D13" s="39"/>
@@ -1581,7 +1564,7 @@
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="65" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" s="66"/>
       <c r="D15" s="39"/>
@@ -1593,7 +1576,7 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="66"/>
       <c r="D17" s="45"/>
@@ -1605,7 +1588,7 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="62"/>
       <c r="D19" s="39"/>
@@ -1617,23 +1600,17 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="63"/>
       <c r="D21" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="45">
-        <v>200042</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="45">
-        <v>13.5</v>
-      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Revert "creating time sheet"
This reverts commit 4ce7a23c54e0495dbb3db4a7cb5f5b9b6098916c.
</commit_message>
<xml_diff>
--- a/public/Format.xlsx
+++ b/public/Format.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D5D19-BD89-4F66-BF9A-640DF04C5E2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1EAB0C-EF71-48AC-B7C1-2EF2E7662421}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily_History" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -214,61 +214,15 @@
   <si>
     <t>名前</t>
   </si>
-  <si>
-    <t>タイムシート</t>
-  </si>
-  <si>
-    <t>氏名：</t>
-  </si>
-  <si>
-    <t>曜日</t>
-  </si>
-  <si>
-    <t>始業時間</t>
-  </si>
-  <si>
-    <t>終了時刻</t>
-  </si>
-  <si>
-    <t>休憩時間</t>
-  </si>
-  <si>
-    <t>実労働時間合計</t>
-  </si>
-  <si>
-    <t>休日出勤</t>
-  </si>
-  <si>
-    <t>深夜勤務</t>
-  </si>
-  <si>
-    <t>備考</t>
-  </si>
-  <si>
-    <t>実労働時間合計：</t>
-  </si>
-  <si>
-    <t>標準労働時間</t>
-  </si>
-  <si>
-    <t>実労働時間</t>
-  </si>
-  <si>
-    <t>差引時間</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
-    <numFmt numFmtId="165" formatCode="d&quot;日&quot;"/>
-    <numFmt numFmtId="166" formatCode="yyyy&quot;年&quot;m&quot;月&quot;dd&quot;日&quot;"/>
-    <numFmt numFmtId="167" formatCode="[Red][=1]aaa;[Blue][=7]aaa;aaa"/>
-    <numFmt numFmtId="168" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -340,41 +294,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -414,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -734,98 +653,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -841,7 +668,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -983,87 +810,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1129,218 +875,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="12" name="Group 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09B3CC83-1783-4D11-B2A3-FF5258B74D89}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr>
-          <a:grpSpLocks/>
-        </xdr:cNvGrpSpPr>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4175760" y="0"/>
-          <a:ext cx="1790700" cy="792480"/>
-          <a:chOff x="617" y="29"/>
-          <a:chExt cx="155" cy="74"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="13" name="Rectangle 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44393A56-59F3-4954-8081-9FFC7F6B5DC0}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr>
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="617" y="29"/>
-            <a:ext cx="75" cy="74"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFFFFF"/>
-          </a:solidFill>
-          <a:ln w="6350">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="14" name="Text Box 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E4ACAE-84EF-4F05-B777-20FAE53F2997}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1">
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="617" y="29"/>
-            <a:ext cx="76" cy="20"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6350">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="ＭＳ Ｐゴシック"/>
-                <a:ea typeface="ＭＳ Ｐゴシック"/>
-              </a:rPr>
-              <a:t>所属長</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="15" name="Rectangle 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A0B2D85-327F-4916-B1DB-05D091188A38}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr>
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="696" y="29"/>
-            <a:ext cx="76" cy="74"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFFFFF"/>
-          </a:solidFill>
-          <a:ln w="6350">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="16" name="Text Box 8">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3D1505A-AB00-4BA2-A613-B44ABABAD015}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1">
-            <a:spLocks noChangeArrowheads="1"/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="696" y="29"/>
-            <a:ext cx="76" cy="21"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6350">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:miter lim="800000"/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr" rtl="0">
-              <a:defRPr sz="1000"/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="ＭＳ Ｐゴシック"/>
-                <a:ea typeface="ＭＳ Ｐゴシック"/>
-              </a:rPr>
-              <a:t>申請者</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1770,38 +1304,38 @@
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="58" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="87" t="s">
+      <c r="H3" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="87" t="s">
+      <c r="I3" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="81" t="s">
+      <c r="J3" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="82"/>
+      <c r="K3" s="55"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="84"/>
-      <c r="C4" s="86"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
       <c r="J4" s="8" t="s">
         <v>22</v>
       </c>
@@ -1854,12 +1388,12 @@
       <c r="G7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="79"/>
-      <c r="J7" s="79"/>
-      <c r="K7" s="80"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="53"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="B8" s="16"/>
@@ -1905,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G22"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1917,18 +1451,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="2:7">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="91"/>
+      <c r="C2" s="64"/>
       <c r="D2" s="29"/>
     </row>
     <row r="3" spans="2:7">
@@ -2017,10 +1551,10 @@
       <c r="D11" s="35"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="89"/>
+      <c r="C13" s="62"/>
       <c r="D13" s="39"/>
     </row>
     <row r="14" spans="2:7">
@@ -2029,10 +1563,10 @@
       <c r="D14" s="42"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="93"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="39"/>
     </row>
     <row r="16" spans="2:7">
@@ -2041,10 +1575,10 @@
       <c r="D16" s="44"/>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="93"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="45"/>
     </row>
     <row r="18" spans="2:4">
@@ -2053,10 +1587,10 @@
       <c r="D18" s="44"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="89"/>
+      <c r="C19" s="62"/>
       <c r="D19" s="39"/>
     </row>
     <row r="20" spans="2:4">
@@ -2065,10 +1599,10 @@
       <c r="D20" s="47"/>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="89" t="s">
+      <c r="B21" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="90"/>
+      <c r="C21" s="63"/>
       <c r="D21" s="48" t="s">
         <v>42</v>
       </c>
@@ -2107,601 +1641,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42507963-C665-4871-BB93-2B59F71CEE46}">
-  <dimension ref="B1:J38"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
-  <cols>
-    <col min="1" max="1" width="0.77734375" style="54" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" style="54" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="54" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="54" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="54" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" style="54" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" style="54" customWidth="1"/>
-    <col min="8" max="9" width="10.77734375" style="54" customWidth="1"/>
-    <col min="10" max="10" width="8.109375" style="54" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="54"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:10" ht="19.2" customHeight="1" thickBot="1">
-      <c r="B1" s="51" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" ht="21.6" customHeight="1" thickBot="1">
-      <c r="B2" s="64">
-        <v>43831</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" ht="19.2" customHeight="1">
-      <c r="B3" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="55"/>
-    </row>
-    <row r="4" spans="2:10" ht="3" customHeight="1"/>
-    <row r="5" spans="2:10" ht="13.8" thickBot="1">
-      <c r="B5" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="53" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="21.6" customHeight="1" thickTop="1">
-      <c r="B6" s="63">
-        <f>B2</f>
-        <v>43831</v>
-      </c>
-      <c r="C6" s="65">
-        <f>WEEKDAY(B6)</f>
-        <v>4</v>
-      </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-    </row>
-    <row r="7" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B7" s="63">
-        <f>B6+1</f>
-        <v>43832</v>
-      </c>
-      <c r="C7" s="65">
-        <f t="shared" ref="C7:C32" si="0">WEEKDAY(B7)</f>
-        <v>5</v>
-      </c>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-    </row>
-    <row r="8" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B8" s="63">
-        <f t="shared" ref="B8:B32" si="1">B7+1</f>
-        <v>43833</v>
-      </c>
-      <c r="C8" s="65">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-    </row>
-    <row r="9" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B9" s="63">
-        <f t="shared" si="1"/>
-        <v>43834</v>
-      </c>
-      <c r="C9" s="65">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-    </row>
-    <row r="10" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B10" s="63">
-        <f t="shared" si="1"/>
-        <v>43835</v>
-      </c>
-      <c r="C10" s="65">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-    </row>
-    <row r="11" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B11" s="63">
-        <f t="shared" si="1"/>
-        <v>43836</v>
-      </c>
-      <c r="C11" s="65">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-    </row>
-    <row r="12" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B12" s="63">
-        <f t="shared" si="1"/>
-        <v>43837</v>
-      </c>
-      <c r="C12" s="65">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-    </row>
-    <row r="13" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B13" s="63">
-        <f t="shared" si="1"/>
-        <v>43838</v>
-      </c>
-      <c r="C13" s="65">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
-    </row>
-    <row r="14" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B14" s="63">
-        <f t="shared" si="1"/>
-        <v>43839</v>
-      </c>
-      <c r="C14" s="65">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
-    </row>
-    <row r="15" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B15" s="63">
-        <f t="shared" si="1"/>
-        <v>43840</v>
-      </c>
-      <c r="C15" s="65">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-    </row>
-    <row r="16" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B16" s="63">
-        <f t="shared" si="1"/>
-        <v>43841</v>
-      </c>
-      <c r="C16" s="65">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-    </row>
-    <row r="17" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B17" s="63">
-        <f t="shared" si="1"/>
-        <v>43842</v>
-      </c>
-      <c r="C17" s="65">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-    </row>
-    <row r="18" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B18" s="63">
-        <f t="shared" si="1"/>
-        <v>43843</v>
-      </c>
-      <c r="C18" s="65">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-    </row>
-    <row r="19" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B19" s="63">
-        <f t="shared" si="1"/>
-        <v>43844</v>
-      </c>
-      <c r="C19" s="65">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-    </row>
-    <row r="20" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B20" s="63">
-        <f t="shared" si="1"/>
-        <v>43845</v>
-      </c>
-      <c r="C20" s="65">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D20" s="75"/>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-    </row>
-    <row r="21" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B21" s="63">
-        <f t="shared" si="1"/>
-        <v>43846</v>
-      </c>
-      <c r="C21" s="65">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-    </row>
-    <row r="22" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B22" s="63">
-        <f t="shared" si="1"/>
-        <v>43847</v>
-      </c>
-      <c r="C22" s="65">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D22" s="75"/>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-    </row>
-    <row r="23" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B23" s="63">
-        <f t="shared" si="1"/>
-        <v>43848</v>
-      </c>
-      <c r="C23" s="65">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D23" s="75"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-    </row>
-    <row r="24" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B24" s="63">
-        <f t="shared" si="1"/>
-        <v>43849</v>
-      </c>
-      <c r="C24" s="65">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-    </row>
-    <row r="25" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B25" s="63">
-        <f t="shared" si="1"/>
-        <v>43850</v>
-      </c>
-      <c r="C25" s="65">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-    </row>
-    <row r="26" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B26" s="63">
-        <f t="shared" si="1"/>
-        <v>43851</v>
-      </c>
-      <c r="C26" s="65">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-    </row>
-    <row r="27" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B27" s="63">
-        <f t="shared" si="1"/>
-        <v>43852</v>
-      </c>
-      <c r="C27" s="65">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-    </row>
-    <row r="28" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B28" s="63">
-        <f t="shared" si="1"/>
-        <v>43853</v>
-      </c>
-      <c r="C28" s="65">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D28" s="75"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-    </row>
-    <row r="29" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B29" s="63">
-        <f t="shared" si="1"/>
-        <v>43854</v>
-      </c>
-      <c r="C29" s="65">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D29" s="75"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-    </row>
-    <row r="30" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B30" s="63">
-        <f t="shared" si="1"/>
-        <v>43855</v>
-      </c>
-      <c r="C30" s="65">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-    </row>
-    <row r="31" spans="2:10" ht="22.2" customHeight="1">
-      <c r="B31" s="63">
-        <f t="shared" si="1"/>
-        <v>43856</v>
-      </c>
-      <c r="C31" s="65">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-    </row>
-    <row r="32" spans="2:10" ht="21.6" customHeight="1">
-      <c r="B32" s="63">
-        <f t="shared" si="1"/>
-        <v>43857</v>
-      </c>
-      <c r="C32" s="65">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-    </row>
-    <row r="33" spans="2:10" ht="21.6" customHeight="1" thickBot="1">
-      <c r="B33" s="72">
-        <f>B32+1</f>
-        <v>43858</v>
-      </c>
-      <c r="C33" s="73">
-        <f>WEEKDAY(B33)</f>
-        <v>3</v>
-      </c>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="66"/>
-    </row>
-    <row r="34" spans="2:10" ht="21.6" customHeight="1" thickTop="1">
-      <c r="B34" s="67"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="69">
-        <v>22</v>
-      </c>
-      <c r="E34" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="68"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="71"/>
-    </row>
-    <row r="35" spans="2:10" ht="7.2" customHeight="1"/>
-    <row r="36" spans="2:10" ht="22.2" customHeight="1" thickBot="1">
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-    </row>
-    <row r="37" spans="2:10" ht="7.2" customHeight="1" thickTop="1"/>
-    <row r="38" spans="2:10" ht="27" customHeight="1">
-      <c r="B38" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="61"/>
-      <c r="D38" s="61">
-        <v>165</v>
-      </c>
-      <c r="E38" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="61">
-        <v>176</v>
-      </c>
-      <c r="G38" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="H38" s="61">
-        <v>11</v>
-      </c>
-      <c r="I38" s="62"/>
-      <c r="J38" s="59"/>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Revert "creating time sheet""
This reverts commit e447b158165dc431854f1004d81b5bf9f9bd3902.
</commit_message>
<xml_diff>
--- a/public/Format.xlsx
+++ b/public/Format.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1EAB0C-EF71-48AC-B7C1-2EF2E7662421}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10D5D19-BD89-4F66-BF9A-640DF04C5E2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily_History" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -214,15 +214,61 @@
   <si>
     <t>名前</t>
   </si>
+  <si>
+    <t>タイムシート</t>
+  </si>
+  <si>
+    <t>氏名：</t>
+  </si>
+  <si>
+    <t>曜日</t>
+  </si>
+  <si>
+    <t>始業時間</t>
+  </si>
+  <si>
+    <t>終了時刻</t>
+  </si>
+  <si>
+    <t>休憩時間</t>
+  </si>
+  <si>
+    <t>実労働時間合計</t>
+  </si>
+  <si>
+    <t>休日出勤</t>
+  </si>
+  <si>
+    <t>深夜勤務</t>
+  </si>
+  <si>
+    <t>備考</t>
+  </si>
+  <si>
+    <t>実労働時間合計：</t>
+  </si>
+  <si>
+    <t>標準労働時間</t>
+  </si>
+  <si>
+    <t>実労働時間</t>
+  </si>
+  <si>
+    <t>差引時間</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="165" formatCode="d&quot;日&quot;"/>
+    <numFmt numFmtId="166" formatCode="yyyy&quot;年&quot;m&quot;月&quot;dd&quot;日&quot;"/>
+    <numFmt numFmtId="167" formatCode="[Red][=1]aaa;[Blue][=7]aaa;aaa"/>
+    <numFmt numFmtId="168" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +340,41 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -333,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -653,6 +734,98 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -668,7 +841,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -810,6 +983,87 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="13" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -875,6 +1129,218 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="12" name="Group 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09B3CC83-1783-4D11-B2A3-FF5258B74D89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4175760" y="0"/>
+          <a:ext cx="1790700" cy="792480"/>
+          <a:chOff x="617" y="29"/>
+          <a:chExt cx="155" cy="74"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="13" name="Rectangle 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44393A56-59F3-4954-8081-9FFC7F6B5DC0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr>
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="617" y="29"/>
+            <a:ext cx="75" cy="74"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:ln w="6350">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="Text Box 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E4ACAE-84EF-4F05-B777-20FAE53F2997}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="617" y="29"/>
+            <a:ext cx="76" cy="20"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="ＭＳ Ｐゴシック"/>
+                <a:ea typeface="ＭＳ Ｐゴシック"/>
+              </a:rPr>
+              <a:t>所属長</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="15" name="Rectangle 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A0B2D85-327F-4916-B1DB-05D091188A38}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr>
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="696" y="29"/>
+            <a:ext cx="76" cy="74"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:ln w="6350">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="16" name="Text Box 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3D1505A-AB00-4BA2-A613-B44ABABAD015}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1">
+            <a:spLocks noChangeArrowheads="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="696" y="29"/>
+            <a:ext cx="76" cy="21"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="6350">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:miter lim="800000"/>
+            <a:headEnd/>
+            <a:tailEnd/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="ＭＳ Ｐゴシック"/>
+                <a:ea typeface="ＭＳ Ｐゴシック"/>
+              </a:rPr>
+              <a:t>申請者</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1304,38 +1770,38 @@
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="85" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="60" t="s">
+      <c r="H3" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="60" t="s">
+      <c r="I3" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="55"/>
+      <c r="K3" s="82"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B4" s="57"/>
-      <c r="C4" s="59"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="86"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
       <c r="J4" s="8" t="s">
         <v>22</v>
       </c>
@@ -1388,12 +1854,12 @@
       <c r="G7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="H7" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="53"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="80"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="B8" s="16"/>
@@ -1439,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1451,18 +1917,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="2:7">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="64"/>
+      <c r="C2" s="91"/>
       <c r="D2" s="29"/>
     </row>
     <row r="3" spans="2:7">
@@ -1551,10 +2017,10 @@
       <c r="D11" s="35"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="62"/>
+      <c r="C13" s="89"/>
       <c r="D13" s="39"/>
     </row>
     <row r="14" spans="2:7">
@@ -1563,10 +2029,10 @@
       <c r="D14" s="42"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="66"/>
+      <c r="C15" s="93"/>
       <c r="D15" s="39"/>
     </row>
     <row r="16" spans="2:7">
@@ -1575,10 +2041,10 @@
       <c r="D16" s="44"/>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="66"/>
+      <c r="C17" s="93"/>
       <c r="D17" s="45"/>
     </row>
     <row r="18" spans="2:4">
@@ -1587,10 +2053,10 @@
       <c r="D18" s="44"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="62"/>
+      <c r="C19" s="89"/>
       <c r="D19" s="39"/>
     </row>
     <row r="20" spans="2:4">
@@ -1599,10 +2065,10 @@
       <c r="D20" s="47"/>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="63"/>
+      <c r="C21" s="90"/>
       <c r="D21" s="48" t="s">
         <v>42</v>
       </c>
@@ -1641,12 +2107,601 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42507963-C665-4871-BB93-2B59F71CEE46}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="0.77734375" style="54" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="54" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="54" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="54" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" style="54" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="54" customWidth="1"/>
+    <col min="8" max="9" width="10.77734375" style="54" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" style="54" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="54"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="19.2" customHeight="1" thickBot="1">
+      <c r="B1" s="51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="21.6" customHeight="1" thickBot="1">
+      <c r="B2" s="64">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="19.2" customHeight="1">
+      <c r="B3" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="55"/>
+    </row>
+    <row r="4" spans="2:10" ht="3" customHeight="1"/>
+    <row r="5" spans="2:10" ht="13.8" thickBot="1">
+      <c r="B5" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="21.6" customHeight="1" thickTop="1">
+      <c r="B6" s="63">
+        <f>B2</f>
+        <v>43831</v>
+      </c>
+      <c r="C6" s="65">
+        <f>WEEKDAY(B6)</f>
+        <v>4</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+    </row>
+    <row r="7" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B7" s="63">
+        <f>B6+1</f>
+        <v>43832</v>
+      </c>
+      <c r="C7" s="65">
+        <f t="shared" ref="C7:C32" si="0">WEEKDAY(B7)</f>
+        <v>5</v>
+      </c>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+    </row>
+    <row r="8" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B8" s="63">
+        <f t="shared" ref="B8:B32" si="1">B7+1</f>
+        <v>43833</v>
+      </c>
+      <c r="C8" s="65">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+    </row>
+    <row r="9" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B9" s="63">
+        <f t="shared" si="1"/>
+        <v>43834</v>
+      </c>
+      <c r="C9" s="65">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+    </row>
+    <row r="10" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B10" s="63">
+        <f t="shared" si="1"/>
+        <v>43835</v>
+      </c>
+      <c r="C10" s="65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+    </row>
+    <row r="11" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B11" s="63">
+        <f t="shared" si="1"/>
+        <v>43836</v>
+      </c>
+      <c r="C11" s="65">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+    </row>
+    <row r="12" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B12" s="63">
+        <f t="shared" si="1"/>
+        <v>43837</v>
+      </c>
+      <c r="C12" s="65">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="74"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+    </row>
+    <row r="13" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B13" s="63">
+        <f t="shared" si="1"/>
+        <v>43838</v>
+      </c>
+      <c r="C13" s="65">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+    </row>
+    <row r="14" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B14" s="63">
+        <f t="shared" si="1"/>
+        <v>43839</v>
+      </c>
+      <c r="C14" s="65">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+    </row>
+    <row r="15" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B15" s="63">
+        <f t="shared" si="1"/>
+        <v>43840</v>
+      </c>
+      <c r="C15" s="65">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+    </row>
+    <row r="16" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B16" s="63">
+        <f t="shared" si="1"/>
+        <v>43841</v>
+      </c>
+      <c r="C16" s="65">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+    </row>
+    <row r="17" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B17" s="63">
+        <f t="shared" si="1"/>
+        <v>43842</v>
+      </c>
+      <c r="C17" s="65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+    </row>
+    <row r="18" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B18" s="63">
+        <f t="shared" si="1"/>
+        <v>43843</v>
+      </c>
+      <c r="C18" s="65">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+    </row>
+    <row r="19" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B19" s="63">
+        <f t="shared" si="1"/>
+        <v>43844</v>
+      </c>
+      <c r="C19" s="65">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+    </row>
+    <row r="20" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B20" s="63">
+        <f t="shared" si="1"/>
+        <v>43845</v>
+      </c>
+      <c r="C20" s="65">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D20" s="75"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
+    </row>
+    <row r="21" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B21" s="63">
+        <f t="shared" si="1"/>
+        <v>43846</v>
+      </c>
+      <c r="C21" s="65">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
+    </row>
+    <row r="22" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B22" s="63">
+        <f t="shared" si="1"/>
+        <v>43847</v>
+      </c>
+      <c r="C22" s="65">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+    </row>
+    <row r="23" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B23" s="63">
+        <f t="shared" si="1"/>
+        <v>43848</v>
+      </c>
+      <c r="C23" s="65">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+    </row>
+    <row r="24" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B24" s="63">
+        <f t="shared" si="1"/>
+        <v>43849</v>
+      </c>
+      <c r="C24" s="65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+    </row>
+    <row r="25" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B25" s="63">
+        <f t="shared" si="1"/>
+        <v>43850</v>
+      </c>
+      <c r="C25" s="65">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+    </row>
+    <row r="26" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B26" s="63">
+        <f t="shared" si="1"/>
+        <v>43851</v>
+      </c>
+      <c r="C26" s="65">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="58"/>
+    </row>
+    <row r="27" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B27" s="63">
+        <f t="shared" si="1"/>
+        <v>43852</v>
+      </c>
+      <c r="C27" s="65">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+    </row>
+    <row r="28" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B28" s="63">
+        <f t="shared" si="1"/>
+        <v>43853</v>
+      </c>
+      <c r="C28" s="65">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D28" s="75"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+    </row>
+    <row r="29" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B29" s="63">
+        <f t="shared" si="1"/>
+        <v>43854</v>
+      </c>
+      <c r="C29" s="65">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+    </row>
+    <row r="30" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B30" s="63">
+        <f t="shared" si="1"/>
+        <v>43855</v>
+      </c>
+      <c r="C30" s="65">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+    </row>
+    <row r="31" spans="2:10" ht="22.2" customHeight="1">
+      <c r="B31" s="63">
+        <f t="shared" si="1"/>
+        <v>43856</v>
+      </c>
+      <c r="C31" s="65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+    </row>
+    <row r="32" spans="2:10" ht="21.6" customHeight="1">
+      <c r="B32" s="63">
+        <f t="shared" si="1"/>
+        <v>43857</v>
+      </c>
+      <c r="C32" s="65">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+    </row>
+    <row r="33" spans="2:10" ht="21.6" customHeight="1" thickBot="1">
+      <c r="B33" s="72">
+        <f>B32+1</f>
+        <v>43858</v>
+      </c>
+      <c r="C33" s="73">
+        <f>WEEKDAY(B33)</f>
+        <v>3</v>
+      </c>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+    </row>
+    <row r="34" spans="2:10" ht="21.6" customHeight="1" thickTop="1">
+      <c r="B34" s="67"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="69">
+        <v>22</v>
+      </c>
+      <c r="E34" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="68"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="71"/>
+    </row>
+    <row r="35" spans="2:10" ht="7.2" customHeight="1"/>
+    <row r="36" spans="2:10" ht="22.2" customHeight="1" thickBot="1">
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+    </row>
+    <row r="37" spans="2:10" ht="7.2" customHeight="1" thickTop="1"/>
+    <row r="38" spans="2:10" ht="27" customHeight="1">
+      <c r="B38" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61">
+        <v>165</v>
+      </c>
+      <c r="E38" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="61">
+        <v>176</v>
+      </c>
+      <c r="G38" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="61">
+        <v>11</v>
+      </c>
+      <c r="I38" s="62"/>
+      <c r="J38" s="59"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>